<commit_message>
Update 05_Trần Tiên Ngọc Yến_KHTT.xlsx
</commit_message>
<xml_diff>
--- a/05. Ngọc Yến/05_Trần Tiên Ngọc Yến_KHTT.xlsx
+++ b/05. Ngọc Yến/05_Trần Tiên Ngọc Yến_KHTT.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan detail" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="93">
   <si>
     <t>QA Training Schedule</t>
   </si>
@@ -119,12 +119,239 @@
 + Chuyển đổi trạng thái
 ...</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>Day One</t>
+  </si>
+  <si>
+    <t>Thứ 4, ngày 16-06-2021</t>
+  </si>
+  <si>
+    <t>Present: Overview about Software Testing
+1. Vòng đời phát triển phần mềm (chú ý focus vào thác nước, V model, Scrum) 
+2. Quy trình kiểm thử phần mềm, 7 nguyên lý kiểm thử phần mềm 
+3. Test level, test type, test method 
+4. Test design technique, black box testing technique (chỉ cần phân loại và nêu được khái niệm, chưa cần đi vào chi tiết) 
+5. Test case, bug report (chỉ cần nêu được khái niệm cơ bản)</t>
+  </si>
+  <si>
+    <t>Southern</t>
+  </si>
+  <si>
+    <t>3h-4h30</t>
+  </si>
+  <si>
+    <t>Bacth 46 present</t>
+  </si>
+  <si>
+    <t>Thứ 5 ngày 17-06-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present (2)
+</t>
+  </si>
+  <si>
+    <t>Booth2</t>
+  </si>
+  <si>
+    <t>16-16h45</t>
+  </si>
+  <si>
+    <t>Loi VT</t>
+  </si>
+  <si>
+    <t>Thứ 6 ngày 18-06-2021</t>
+  </si>
+  <si>
+    <t>Lecture : Requirement Analysis + Q&amp;A file</t>
+  </si>
+  <si>
+    <t>Booth1</t>
+  </si>
+  <si>
+    <t>10-12h</t>
+  </si>
+  <si>
+    <t>Thứ 2 ngày 21/06/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OE46: REVIEW practice Q&amp;A file
+</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/eeq-uxje-hrp</t>
+  </si>
+  <si>
+    <t>2:00 – 3:00PM</t>
+  </si>
+  <si>
+    <t>Thứ 3 ngày 22/06/2021</t>
+  </si>
+  <si>
+    <t>Lecture test design techique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://meet.google.com/swf-frax-znz
+</t>
+  </si>
+  <si>
+    <t>8:30 – 10:30AM</t>
+  </si>
+  <si>
+    <t>Tự tìm hiểu</t>
+  </si>
+  <si>
+    <t>Thứ 4 ngày 23/06/2021</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/nur-utfo-haa?authuser=0</t>
+  </si>
+  <si>
+    <t>2-4h</t>
+  </si>
+  <si>
+    <t>Loi VT review</t>
+  </si>
+  <si>
+    <t>Practice 4 : https://sal.vn/ghi4Uo</t>
+  </si>
+  <si>
+    <t>https://sal.vn/ghi4Uo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thứ năm, 24 tháng 6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture: Test checklist
+Practice Create test check list for create new user screen 
+- Nhận specs
+- Đọc hiểu. phân tích , log q/A 
+- Test plan 
+- Test design 
+- Test checklist 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://meet.google.com/hky-ycmi-qsx
+</t>
+  </si>
+  <si>
+    <t>2:00 – 4:00PM</t>
+  </si>
+  <si>
+    <t>LoiVT lecture</t>
+  </si>
+  <si>
+    <t>Review Test design test checklist</t>
+  </si>
+  <si>
+    <t>Review chéo test checklist</t>
+  </si>
+  <si>
+    <t>Review: Test checklist (1)</t>
+  </si>
+  <si>
+    <t>Lecture Test case</t>
+  </si>
+  <si>
+    <t>Lecture: Bug report</t>
+  </si>
+  <si>
+    <t>Review Bug report</t>
+  </si>
+  <si>
+    <t>review Verify bug report</t>
+  </si>
+  <si>
+    <t>Interview Tutorial 1</t>
+  </si>
+  <si>
+    <t>Interview Tutorial 2</t>
+  </si>
+  <si>
+    <t>SQL
+(2 days)</t>
+  </si>
+  <si>
+    <t>Join lecture</t>
+  </si>
+  <si>
+    <t>Thuy BNT</t>
+  </si>
+  <si>
+    <t>Self Study + Practice</t>
+  </si>
+  <si>
+    <t>Self review and practice</t>
+  </si>
+  <si>
+    <t>Review Practice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project 1
+</t>
+  </si>
+  <si>
+    <t>Kick-off</t>
+  </si>
+  <si>
+    <t>Self study spec, Log Q&amp;A</t>
+  </si>
+  <si>
+    <t>Review Test plan</t>
+  </si>
+  <si>
+    <t>Review Test case</t>
+  </si>
+  <si>
+    <t>Scrum
+( 1 days)</t>
+  </si>
+  <si>
+    <t>Scrum</t>
+  </si>
+  <si>
+    <t>Khoang edu</t>
+  </si>
+  <si>
+    <t>9-12h</t>
+  </si>
+  <si>
+    <t>Thao DTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project 2
+</t>
+  </si>
+  <si>
+    <t>Thứ hai, 28 tháng 6⋅
+9:00 – 11:00AM</t>
+  </si>
+  <si>
+    <t>Thứ ba, 29 tháng 6⋅
+9:00 – 11:00AM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,8 +385,49 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,8 +458,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -333,11 +607,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -351,6 +641,27 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -360,29 +671,79 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -684,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -728,31 +1089,31 @@
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" ht="21.75" customHeight="1" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -760,65 +1121,65 @@
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="115.5" customHeight="1" thickBot="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="99" customHeight="1" thickBot="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="105.75" customHeight="1" thickBot="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -832,13 +1193,537 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="15"/>
+    <col min="3" max="3" width="16.28515625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" style="15" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15">
+      <c r="A1" s="32"/>
+      <c r="B1" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="36"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="1:7" ht="200.25" customHeight="1">
+      <c r="A3" s="37"/>
+      <c r="B3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="27" customHeight="1">
+      <c r="A4" s="37"/>
+      <c r="B4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="33" customHeight="1">
+      <c r="A5" s="37"/>
+      <c r="B5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30.75" customHeight="1">
+      <c r="A6" s="37"/>
+      <c r="B6" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" ht="30.75" customHeight="1">
+      <c r="A7" s="37"/>
+      <c r="B7" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="33" customHeight="1">
+      <c r="A8" s="37"/>
+      <c r="B8" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1">
+      <c r="A9" s="37"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" ht="117.75" customHeight="1">
+      <c r="A10" s="37"/>
+      <c r="B10" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="33.75" customHeight="1">
+      <c r="A11" s="37"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" ht="36.75" customHeight="1">
+      <c r="A12" s="37"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" ht="33" customHeight="1">
+      <c r="A13" s="37"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" ht="36" customHeight="1">
+      <c r="A14" s="37"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" spans="1:7" ht="33" customHeight="1">
+      <c r="A15" s="37"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="16" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A16" s="37"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" spans="1:7" ht="38.25" customHeight="1">
+      <c r="A17" s="37"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" spans="1:7" ht="33" customHeight="1">
+      <c r="A18" s="37"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" spans="1:7" ht="34.5" customHeight="1">
+      <c r="A19" s="37"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A20" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.5" customHeight="1">
+      <c r="A21" s="37"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="27.75" customHeight="1">
+      <c r="A22" s="37"/>
+      <c r="B22" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="21" customHeight="1">
+      <c r="A23" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A24" s="37"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+    </row>
+    <row r="25" spans="1:7" ht="18" customHeight="1">
+      <c r="A25" s="37"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+    </row>
+    <row r="26" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A26" s="37"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+    </row>
+    <row r="27" spans="1:7" ht="18" customHeight="1">
+      <c r="A27" s="37"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A28" s="37"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+    </row>
+    <row r="29" spans="1:7" ht="30.75" customHeight="1">
+      <c r="A29" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="37"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="37"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="37"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="37"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="37"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" display="https://maps.google.com/maps?hl=vi&amp;q=DN-FT-4F-Southern%20%286%29&amp;source=calendar"/>
+    <hyperlink ref="E6" r:id="rId2"/>
+    <hyperlink ref="E7" r:id="rId3" display="https://meet.google.com/swf-frax-znz"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="D9" r:id="rId5" display="https://sal.vn/ghi4Uo"/>
+    <hyperlink ref="E9" r:id="rId6"/>
+    <hyperlink ref="E10" r:id="rId7" display="https://meet.google.com/hky-ycmi-qsx"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>